<commit_message>
new file:   GRU model.md
</commit_message>
<xml_diff>
--- a/data_feature.xlsx
+++ b/data_feature.xlsx
@@ -743,7 +743,7 @@
         <v>0.4</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -812,7 +812,7 @@
         <v>0.4</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1157,7 +1157,7 @@
         <v>0.4</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1318,7 +1318,7 @@
         <v>0.4</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1502,7 +1502,7 @@
         <v>0.8</v>
       </c>
       <c r="G46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -2261,7 +2261,7 @@
         <v>0.8</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -2468,7 +2468,7 @@
         <v>0.4</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -2905,7 +2905,7 @@
         <v>0.4</v>
       </c>
       <c r="G107" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -2974,7 +2974,7 @@
         <v>0.4</v>
       </c>
       <c r="G110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
@@ -3089,7 +3089,7 @@
         <v>0.8</v>
       </c>
       <c r="G115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -3250,7 +3250,7 @@
         <v>0.4</v>
       </c>
       <c r="G122" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
@@ -3342,7 +3342,7 @@
         <v>0.4</v>
       </c>
       <c r="G126" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
@@ -3572,7 +3572,7 @@
         <v>0.4</v>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -3940,7 +3940,7 @@
         <v>0.4</v>
       </c>
       <c r="G152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -4124,7 +4124,7 @@
         <v>0.8</v>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
@@ -4492,7 +4492,7 @@
         <v>0.4</v>
       </c>
       <c r="G176" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177">
@@ -4722,7 +4722,7 @@
         <v>0.8</v>
       </c>
       <c r="G186" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
@@ -5205,7 +5205,7 @@
         <v>0.4</v>
       </c>
       <c r="G207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208">
@@ -5297,7 +5297,7 @@
         <v>0.4</v>
       </c>
       <c r="G211" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
@@ -5320,7 +5320,7 @@
         <v>0.4</v>
       </c>
       <c r="G212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213">
@@ -5343,7 +5343,7 @@
         <v>0.4</v>
       </c>
       <c r="G213" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -5366,7 +5366,7 @@
         <v>0.4</v>
       </c>
       <c r="G214" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215">
@@ -5550,7 +5550,7 @@
         <v>0.4</v>
       </c>
       <c r="G222" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223">
@@ -5918,7 +5918,7 @@
         <v>0.4</v>
       </c>
       <c r="G238" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="239">
@@ -6148,7 +6148,7 @@
         <v>0.4</v>
       </c>
       <c r="G248" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="249">
@@ -6194,7 +6194,7 @@
         <v>0.4</v>
       </c>
       <c r="G250" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251">
@@ -6447,7 +6447,7 @@
         <v>0.8</v>
       </c>
       <c r="G261" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
@@ -6470,7 +6470,7 @@
         <v>0.4</v>
       </c>
       <c r="G262" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
@@ -6516,7 +6516,7 @@
         <v>0.4</v>
       </c>
       <c r="G264" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -6723,7 +6723,7 @@
         <v>0.4</v>
       </c>
       <c r="G273" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="274">
@@ -6861,7 +6861,7 @@
         <v>0.8</v>
       </c>
       <c r="G279" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="280">
@@ -6976,7 +6976,7 @@
         <v>0.4</v>
       </c>
       <c r="G284" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285">
@@ -7022,7 +7022,7 @@
         <v>0.8</v>
       </c>
       <c r="G286" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="287">
@@ -7045,7 +7045,7 @@
         <v>0.4</v>
       </c>
       <c r="G287" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288">
@@ -7275,7 +7275,7 @@
         <v>0.4</v>
       </c>
       <c r="G297" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="298">
@@ -7321,7 +7321,7 @@
         <v>0.4</v>
       </c>
       <c r="G299" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300">
@@ -7390,7 +7390,7 @@
         <v>0.4</v>
       </c>
       <c r="G302" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="303">
@@ -7528,7 +7528,7 @@
         <v>0.4</v>
       </c>
       <c r="G308" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="309">
@@ -7551,7 +7551,7 @@
         <v>0.4</v>
       </c>
       <c r="G309" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="310">
@@ -7666,7 +7666,7 @@
         <v>0.4</v>
       </c>
       <c r="G314" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315">
@@ -7689,7 +7689,7 @@
         <v>0.4</v>
       </c>
       <c r="G315" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="316">
@@ -7781,7 +7781,7 @@
         <v>0.4</v>
       </c>
       <c r="G319" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320">
@@ -8103,7 +8103,7 @@
         <v>0.4</v>
       </c>
       <c r="G333" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="334">
@@ -8149,7 +8149,7 @@
         <v>0.4</v>
       </c>
       <c r="G335" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="336">
@@ -8494,7 +8494,7 @@
         <v>0.4</v>
       </c>
       <c r="G350" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="351">

</xml_diff>